<commit_message>
Update census data 🙀
</commit_message>
<xml_diff>
--- a/data/georgia_census/adjara/batumi/age_dependency.xlsx
+++ b/data/georgia_census/adjara/batumi/age_dependency.xlsx
@@ -1007,13 +1007,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6131953-B12A-42F1-B339-9F6B48A8FBD2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B05BD2B-CEF6-4807-9335-730DB4E8092E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF79738E-564C-4858-8C3B-9C128B5C7691}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D35AE96-C350-4F68-B18E-519696F33F75}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC798975-7C4E-4643-858D-D594A4D13024}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51AADB85-719B-492F-8F31-4D14FE37F973}"/>
 </file>
</xml_diff>